<commit_message>
update translations - report
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/shinyssdtools/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/poissonconsulting/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCC060C-530E-0E4F-8987-D760782E5360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4FB864-62F3-7441-A3E4-3E03B1C62EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12480" yWindow="500" windowWidth="12460" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="760" windowWidth="33660" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="224">
   <si>
     <t>id</t>
   </si>
@@ -757,6 +757,15 @@
   </si>
   <si>
     <t>Estimation nécessaire</t>
+  </si>
+  <si>
+    <t>nav5</t>
+  </si>
+  <si>
+    <t>4. Report</t>
+  </si>
+  <si>
+    <t>4. Rapport</t>
   </si>
 </sst>
 </file>
@@ -2137,10 +2146,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU79"/>
+  <dimension ref="A1:IU80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2209,791 +2218,802 @@
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
+      <c r="B6" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>221</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>211</v>
+        <v>58</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>219</v>
+        <v>70</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>219</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>79</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>218</v>
+        <v>92</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>216</v>
+        <v>95</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>220</v>
+        <v>217</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>98</v>
+        <v>216</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>213</v>
+        <v>165</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B77" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C77" s="8" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
+    <row r="80" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B64" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C64" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
+    <hyperlink ref="B65" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C65" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
ensure that french translation works for downloads
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/poissonconsulting/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F78BD6-9909-7B4D-A70A-C4BF4CFC854D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88B4272-2995-CC42-88CB-7117753654AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="760" windowWidth="33660" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="231">
   <si>
     <t>id</t>
   </si>
@@ -775,6 +775,18 @@
   </si>
   <si>
     <t>R Code</t>
+  </si>
+  <si>
+    <t>Dpi</t>
+  </si>
+  <si>
+    <t>2download</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>Télécharger</t>
   </si>
 </sst>
 </file>
@@ -2155,10 +2167,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU81"/>
+  <dimension ref="A1:IU82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2478,562 +2490,573 @@
     </row>
     <row r="29" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>76</v>
+        <v>228</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>215</v>
+        <v>89</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>213</v>
+        <v>92</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>95</v>
+        <v>213</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>210</v>
+        <v>162</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B79" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C79" s="8" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="81" spans="2:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
+    <row r="82" spans="2:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B66" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C66" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
+    <hyperlink ref="B67" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C67" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
add csv and xlsx file translations
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/poissonconsulting/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A1F208-A2E9-474D-AA85-AAA04C8ABA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAF7DF4-9E89-304A-977D-BD2BC647979A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="760" windowWidth="33660" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="236">
   <si>
     <t>id</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>2dlplot</t>
-  </si>
-  <si>
-    <t>2dltable</t>
   </si>
   <si>
     <t>3est</t>
@@ -793,6 +790,18 @@
   </si>
   <si>
     <t>Click 'Get CL' to calculate the upper and lower confidence limits (CL) for the estimated hazard concentration and selected % threshold.</t>
+  </si>
+  <si>
+    <t>2dlxlsx</t>
+  </si>
+  <si>
+    <t>2dlcsv</t>
+  </si>
+  <si>
+    <t>XLSX File</t>
+  </si>
+  <si>
+    <t>Fichier XLSX</t>
   </si>
 </sst>
 </file>
@@ -2173,10 +2182,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU83"/>
+  <dimension ref="A1:IU84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2246,18 +2255,18 @@
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>16</v>
@@ -2265,13 +2274,13 @@
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>211</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2345,10 +2354,10 @@
         <v>35</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>214</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2411,10 +2420,10 @@
         <v>51</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>221</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2436,7 +2445,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2444,10 +2453,10 @@
         <v>57</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2488,21 +2497,21 @@
         <v>67</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="12" t="s">
         <v>219</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2532,21 +2541,21 @@
         <v>74</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>228</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2554,526 +2563,537 @@
         <v>77</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>223</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>78</v>
+        <v>232</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>81</v>
+        <v>233</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>205</v>
+        <v>81</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>207</v>
+      <c r="C39" s="12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>88</v>
+        <v>202</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>231</v>
+        <v>97</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>232</v>
+        <v>101</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>142</v>
+        <v>137</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>145</v>
+        <v>140</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>200</v>
+        <v>152</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B81" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="C81" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C80" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
+    </row>
+    <row r="84" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B68" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C68" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
+    <hyperlink ref="B69" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C69" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
translations working for renderUI inputs, sidebar width
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/poissonconsulting/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCAD072-0282-C843-81A1-1E5B206D6AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800BCC93-2DF3-524C-81D1-9DAE322A3ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="760" windowWidth="33660" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - translations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="257">
   <si>
     <t>id</t>
   </si>
@@ -289,30 +302,12 @@
     <t>3label</t>
   </si>
   <si>
-    <t>Label by:</t>
-  </si>
-  <si>
-    <t>Organiser les étiquettes par :</t>
-  </si>
-  <si>
     <t>3colour</t>
   </si>
   <si>
-    <t>Colour by:</t>
-  </si>
-  <si>
-    <t>Organiser les couleurs par :</t>
-  </si>
-  <si>
     <t>3symbol</t>
   </si>
   <si>
-    <t>Symbol by:</t>
-  </si>
-  <si>
-    <t>Organiser les symboles par :</t>
-  </si>
-  <si>
     <t>3plotopts</t>
   </si>
   <si>
@@ -337,9 +332,6 @@
     <t>3help</t>
   </si>
   <si>
-    <t xml:space="preserve">Cliquer 'Obtenir bornes' pour obtenir les bornes inférieures et supérieures de l'intervalle de confiance  pour l’estimation de la concentration présentant un risque et le seuil (%) sélectionné. </t>
-  </si>
-  <si>
     <t>3hc</t>
   </si>
   <si>
@@ -467,9 +459,6 @@
   </si>
   <si>
     <t>3cldesc3</t>
-  </si>
-  <si>
-    <t>This will take around</t>
   </si>
   <si>
     <t>Cela prendra environ</t>
@@ -789,9 +778,6 @@
     <t>Options de formatage du fichier PNG</t>
   </si>
   <si>
-    <t>Click 'Get CL' to calculate the upper and lower confidence limits (CL) for the estimated hazard concentration and selected % threshold.</t>
-  </si>
-  <si>
     <t>2dlxlsx</t>
   </si>
   <si>
@@ -829,6 +815,69 @@
   </si>
   <si>
     <t>% des espèces</t>
+  </si>
+  <si>
+    <t>3cl2</t>
+  </si>
+  <si>
+    <t>Confidence limits</t>
+  </si>
+  <si>
+    <t>Bornes de l'intervalle de confiance</t>
+  </si>
+  <si>
+    <t>Click 'Get CL' to calculate the upper and lower confidence limits (CL) for the estimate.</t>
+  </si>
+  <si>
+    <t>Cliquer 'Obtenir bornes' pour obtenir les bornes inférieures et supérieures de l'intervalle de confiance  pour l’estimation.</t>
+  </si>
+  <si>
+    <t>hintcolour</t>
+  </si>
+  <si>
+    <t>Colour variable cannot be numeric.</t>
+  </si>
+  <si>
+    <t>La colonne 'Colour' ne doit pas contenir de nombres.</t>
+  </si>
+  <si>
+    <t>Label by</t>
+  </si>
+  <si>
+    <t>Colour by</t>
+  </si>
+  <si>
+    <t>Symbol by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organiser les étiquettes par </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organiser les couleurs par </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organiser les symboles par </t>
+  </si>
+  <si>
+    <t>It will take around</t>
+  </si>
+  <si>
+    <t>hintconc0</t>
+  </si>
+  <si>
+    <t>hintconcmiss</t>
+  </si>
+  <si>
+    <t>Concentration must not be missing.</t>
+  </si>
+  <si>
+    <t>Concentration must not be 0.</t>
+  </si>
+  <si>
+    <t>La concentration ne doit être manquante.</t>
+  </si>
+  <si>
+    <t>La concentration ne doit pas être zéro.</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1055,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1047,6 +1096,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2209,10 +2261,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU87"/>
+  <dimension ref="A1:IU94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2282,18 +2334,18 @@
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>207</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>215</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>16</v>
@@ -2301,13 +2353,13 @@
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2381,10 +2433,10 @@
         <v>35</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2447,10 +2499,10 @@
         <v>51</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2472,7 +2524,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2480,10 +2532,10 @@
         <v>57</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2524,21 +2576,21 @@
         <v>67</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2568,21 +2620,21 @@
         <v>74</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2590,32 +2642,32 @@
         <v>77</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2645,21 +2697,21 @@
         <v>84</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2677,483 +2729,530 @@
       <c r="A42" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>90</v>
+      <c r="B42" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>105</v>
+        <v>239</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>106</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>117</v>
+        <v>236</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>138</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>141</v>
+        <v>130</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>144</v>
+        <v>133</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>152</v>
+        <v>141</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>250</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>199</v>
+        <v>144</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>158</v>
+        <v>147</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>170</v>
+        <v>251</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>173</v>
+        <v>252</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="6" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>190</v>
+        <v>172</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="6" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="6" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>197</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
+      <c r="A87" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+    </row>
+    <row r="94" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C94" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B72" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C72" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
+    <hyperlink ref="B73" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C73" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
translate new report inputs, preivew pdf before download
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/poissonconsulting/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7471950-AC3D-4443-BD88-52A97C856B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA2C17F-FF68-104B-982F-1884A88C7F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="760" windowWidth="33660" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="272">
   <si>
     <t>id</t>
   </si>
@@ -896,6 +896,33 @@
   </si>
   <si>
     <t>Fichier HTML</t>
+  </si>
+  <si>
+    <t>hintpredict</t>
+  </si>
+  <si>
+    <t>You have not successfully generated predictions yet. Run the 'Predict' tab first.</t>
+  </si>
+  <si>
+    <t>Aucune prédiction n'a encore été générée avec succès. Exécuter d'abord l'onglet 'Estimation'.</t>
+  </si>
+  <si>
+    <t>getreport</t>
+  </si>
+  <si>
+    <t>Get Report</t>
+  </si>
+  <si>
+    <t>Obtenir Rapport</t>
+  </si>
+  <si>
+    <t>prevreport</t>
+  </si>
+  <si>
+    <t>Prévisualiser le rapport</t>
+  </si>
+  <si>
+    <t>Preview report</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1100,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1118,6 +1145,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2279,10 +2309,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU96"/>
+  <dimension ref="A1:IU99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3097,202 +3127,235 @@
     </row>
     <row r="74" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>150</v>
+        <v>266</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>153</v>
+        <v>269</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="B77" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>256</v>
+        <v>151</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>255</v>
+        <v>154</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>159</v>
+        <v>251</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>162</v>
+        <v>252</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>182</v>
+        <v>175</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="6" t="s">
-        <v>241</v>
+        <v>181</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>243</v>
+        <v>182</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B93" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C93" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B93" s="10"/>
-      <c r="C93" s="10"/>
-    </row>
     <row r="96" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C96" s="8"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+    </row>
+    <row r="99" spans="3:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C99" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B75" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C75" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
+    <hyperlink ref="B77" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C77" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
add translation for copy button
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/poissonconsulting/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA2C17F-FF68-104B-982F-1884A88C7F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5FD072-50E7-7A40-82B3-1F65568E562C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="760" windowWidth="33660" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="275">
   <si>
     <t>id</t>
   </si>
@@ -923,6 +923,15 @@
   </si>
   <si>
     <t>Preview report</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>Copier le code</t>
+  </si>
+  <si>
+    <t>Copy code</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1109,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1148,6 +1157,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2309,10 +2324,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU99"/>
+  <dimension ref="A1:IU100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3345,12 +3360,23 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-    </row>
-    <row r="99" spans="3:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C99" s="8"/>
+    <row r="94" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+    </row>
+    <row r="100" spans="2:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C100" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>